<commit_message>
Add: Gant Chart, Schedules, System architecture
</commit_message>
<xml_diff>
--- a/Development Plan/Gant Chart.xlsx
+++ b/Development Plan/Gant Chart.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="10.0" lowestEdited="10.0" rupBuild="0.5152"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ThisWorkbook" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="6750" tabRatio="501"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="17565" windowHeight="6720" tabRatio="501"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -14,82 +14,88 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+  <x:si>
+    <x:t>댓글의 긍정/부정 분석</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>허진수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>토</x:t>
+  </x:si>
+  <x:si>
+    <x:t>금</x:t>
+  </x:si>
+  <x:si>
+    <x:t>김현지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Page 제작</x:t>
+  </x:si>
+  <x:si>
+    <x:t>카드리딘</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2주차 (05.30 ~ 06.05)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1주차 (05.23 ~ 29)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3주차 (06.06 ~ 12)</x:t>
+  </x:si>
   <x:si>
     <x:t>4주차 (06.13 ~ 19)</x:t>
   </x:si>
   <x:si>
-    <x:t>카드리딘</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3주차 (06.06 ~ 12)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>금</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일</x:t>
-  </x:si>
-  <x:si>
-    <x:t>토</x:t>
-  </x:si>
-  <x:si>
-    <x:t>목</x:t>
+    <x:t>카드리딘, 허진수, 김현지, 이연수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Page 디자인</x:t>
+  </x:si>
+  <x:si>
+    <x:t>크롤링한 데이터 관리</x:t>
+  </x:si>
+  <x:si>
+    <x:t>워드 클라우드 제작</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rest API 생성</x:t>
+  </x:si>
+  <x:si>
+    <x:t>영상 댓글 크롤링</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이연수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>월</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알고리즘, 모델 자료 수집</x:t>
   </x:si>
   <x:si>
     <x:t>개발 환경 Setting</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알고리즘, 모델 자료 수집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2주차 (05.30 ~ 06.05)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>김현지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>허진수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1주차 (05.23 ~ 29)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Page 디자인</x:t>
-  </x:si>
-  <x:si>
-    <x:t>크롤링한 데이터 관리</x:t>
-  </x:si>
-  <x:si>
-    <x:t>영상 댓글 크롤링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>워드 클라우드 제작</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rest API 생성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이연수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Page 제작</x:t>
-  </x:si>
-  <x:si>
-    <x:t>월</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="8">
+  <x:fonts count="9">
     <x:font>
       <x:name val="돋움"/>
       <x:sz val="11"/>
@@ -124,6 +130,12 @@
       <x:name val="돋움"/>
       <x:sz val="11"/>
       <x:color rgb="ff000000"/>
+      <x:b val="1"/>
+    </x:font>
+    <x:font>
+      <x:name val="돋움"/>
+      <x:sz val="11"/>
+      <x:color rgb="ffff0000"/>
       <x:b val="1"/>
     </x:font>
     <x:font>
@@ -259,7 +271,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="9">
+  <x:cellXfs count="13">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -288,19 +300,6 @@
       </mc:Choice>
       <mc:Fallback>
         <x:xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-          <x:alignment horizontal="center" vertical="center"/>
-        </x:xf>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
-          <x:alignment horizontal="center" vertical="center"/>
-          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
-        </x:xf>
-      </mc:Choice>
-      <mc:Fallback>
-        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
           <x:alignment horizontal="center" vertical="center"/>
         </x:xf>
       </mc:Fallback>
@@ -357,6 +356,31 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+          <x:alignment horizontal="center" vertical="center"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="6">
     <x:cellStyle xfId="15" builtinId="5" iLevel="0"/>
@@ -372,6 +396,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -454,6 +479,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -488,6 +514,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -532,6 +559,7 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -575,6 +603,7 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -658,8 +687,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
-            <x:color indexed="64"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -670,7 +699,6 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
-            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
         </x:dxf>
@@ -680,8 +708,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
-            <x:color indexed="64"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -697,7 +725,6 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
-            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -712,8 +739,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
-            <x:color indexed="64"/>
             <x:b val="1"/>
+            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -729,7 +756,6 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
-            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -1022,147 +1048,147 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="A1:AC14"/>
+  <x:dimension ref="A1:AC16"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="G12" activeCellId="0" sqref="G12:G12"/>
+      <x:selection activeCell="Q7" activeCellId="0" sqref="Q7:Q7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.550000000000001"/>
   <x:cols>
-    <x:col min="1" max="1" width="24.77734375" customWidth="1"/>
+    <x:col min="1" max="1" width="28.77734375" customWidth="1"/>
     <x:col min="2" max="29" width="4.77734375" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:29">
       <x:c r="A1" s="3"/>
-      <x:c r="B1" s="4" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="C1" s="4"/>
-      <x:c r="D1" s="4"/>
-      <x:c r="E1" s="4"/>
-      <x:c r="F1" s="4"/>
-      <x:c r="G1" s="4"/>
-      <x:c r="H1" s="4"/>
-      <x:c r="I1" s="4" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="J1" s="4"/>
-      <x:c r="K1" s="4"/>
-      <x:c r="L1" s="4"/>
-      <x:c r="M1" s="4"/>
-      <x:c r="N1" s="4"/>
-      <x:c r="O1" s="4"/>
-      <x:c r="P1" s="4" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="Q1" s="4"/>
-      <x:c r="R1" s="4"/>
-      <x:c r="S1" s="4"/>
-      <x:c r="T1" s="4"/>
-      <x:c r="U1" s="4"/>
-      <x:c r="V1" s="4"/>
-      <x:c r="W1" s="4" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="X1" s="4"/>
-      <x:c r="Y1" s="4"/>
-      <x:c r="Z1" s="4"/>
-      <x:c r="AA1" s="4"/>
-      <x:c r="AB1" s="4"/>
-      <x:c r="AC1" s="4"/>
+      <x:c r="B1" s="8" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C1" s="8"/>
+      <x:c r="D1" s="8"/>
+      <x:c r="E1" s="8"/>
+      <x:c r="F1" s="8"/>
+      <x:c r="G1" s="8"/>
+      <x:c r="H1" s="8"/>
+      <x:c r="I1" s="8" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="J1" s="8"/>
+      <x:c r="K1" s="8"/>
+      <x:c r="L1" s="8"/>
+      <x:c r="M1" s="8"/>
+      <x:c r="N1" s="8"/>
+      <x:c r="O1" s="8"/>
+      <x:c r="P1" s="8" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="Q1" s="8"/>
+      <x:c r="R1" s="8"/>
+      <x:c r="S1" s="8"/>
+      <x:c r="T1" s="8"/>
+      <x:c r="U1" s="8"/>
+      <x:c r="V1" s="8"/>
+      <x:c r="W1" s="8" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="X1" s="8"/>
+      <x:c r="Y1" s="8"/>
+      <x:c r="Z1" s="8"/>
+      <x:c r="AA1" s="8"/>
+      <x:c r="AB1" s="8"/>
+      <x:c r="AC1" s="8"/>
     </x:row>
     <x:row r="2" spans="1:29">
       <x:c r="A2" s="1"/>
-      <x:c r="B2" s="5" t="s">
+      <x:c r="B2" s="4" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="C2" s="5" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="D2" s="5" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="E2" s="5" t="s">
+      <x:c r="C2" s="4" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E2" s="4" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="F2" s="5" t="s">
+      <x:c r="F2" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="G2" s="4" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="G2" s="5" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="H2" s="5" t="s">
+      <x:c r="H2" s="4" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="I2" s="5" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="J2" s="5" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K2" s="5" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="L2" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="M2" s="5" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="I2" s="6" t="s">
+      <x:c r="N2" s="5" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="O2" s="5" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="P2" s="6" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="J2" s="6" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="K2" s="6" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="L2" s="6" t="s">
+      <x:c r="Q2" s="6" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="R2" s="6" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="S2" s="6" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="M2" s="6" t="s">
+      <x:c r="T2" s="6" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="U2" s="6" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="N2" s="6" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="O2" s="6" t="s">
+      <x:c r="V2" s="6" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="W2" s="7" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="X2" s="7" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="Y2" s="7" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="Z2" s="7" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="AA2" s="7" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="P2" s="7" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="Q2" s="7" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="R2" s="7" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="S2" s="7" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="T2" s="7" t="s">
+      <x:c r="AB2" s="7" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="U2" s="7" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="V2" s="7" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="W2" s="8" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="X2" s="8" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="Y2" s="8" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="Z2" s="8" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="AA2" s="8" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="AB2" s="8" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="AC2" s="8" t="s">
-        <x:v>4</x:v>
+      <x:c r="AC2" s="7" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:29">
       <x:c r="A3" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="B3" s="1"/>
       <x:c r="C3" s="1"/>
@@ -1195,15 +1221,15 @@
     </x:row>
     <x:row r="4" spans="1:29">
       <x:c r="A4" s="1" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B4" s="3"/>
-      <x:c r="C4" s="3"/>
-      <x:c r="D4" s="3"/>
-      <x:c r="E4" s="3"/>
-      <x:c r="F4" s="3"/>
-      <x:c r="G4" s="3"/>
-      <x:c r="H4" s="3"/>
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B4" s="4"/>
+      <x:c r="C4" s="4"/>
+      <x:c r="D4" s="4"/>
+      <x:c r="E4" s="4"/>
+      <x:c r="F4" s="4"/>
+      <x:c r="G4" s="4"/>
+      <x:c r="H4" s="4"/>
       <x:c r="I4" s="1"/>
       <x:c r="J4" s="1"/>
       <x:c r="K4" s="1"/>
@@ -1228,22 +1254,22 @@
     </x:row>
     <x:row r="5" spans="1:29">
       <x:c r="A5" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B5" s="3"/>
       <x:c r="C5" s="3"/>
-      <x:c r="D5" s="3"/>
-      <x:c r="E5" s="3"/>
-      <x:c r="F5" s="3"/>
-      <x:c r="G5" s="3"/>
-      <x:c r="H5" s="3"/>
-      <x:c r="I5" s="1"/>
-      <x:c r="J5" s="1"/>
-      <x:c r="K5" s="1"/>
-      <x:c r="L5" s="1"/>
-      <x:c r="M5" s="1"/>
-      <x:c r="N5" s="1"/>
-      <x:c r="O5" s="1"/>
+      <x:c r="D5" s="4"/>
+      <x:c r="E5" s="4"/>
+      <x:c r="F5" s="4"/>
+      <x:c r="G5" s="4"/>
+      <x:c r="H5" s="4"/>
+      <x:c r="I5" s="5"/>
+      <x:c r="J5" s="5"/>
+      <x:c r="K5" s="5"/>
+      <x:c r="L5" s="5"/>
+      <x:c r="M5" s="5"/>
+      <x:c r="N5" s="5"/>
+      <x:c r="O5" s="5"/>
       <x:c r="P5" s="1"/>
       <x:c r="Q5" s="1"/>
       <x:c r="R5" s="1"/>
@@ -1261,29 +1287,29 @@
     </x:row>
     <x:row r="6" spans="1:29">
       <x:c r="A6" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B6" s="1"/>
       <x:c r="C6" s="1"/>
       <x:c r="D6" s="1"/>
       <x:c r="E6" s="1"/>
       <x:c r="F6" s="1"/>
-      <x:c r="G6" s="1"/>
-      <x:c r="H6" s="1"/>
-      <x:c r="I6" s="1"/>
-      <x:c r="J6" s="1"/>
-      <x:c r="K6" s="1"/>
-      <x:c r="L6" s="1"/>
-      <x:c r="M6" s="1"/>
-      <x:c r="N6" s="1"/>
-      <x:c r="O6" s="1"/>
-      <x:c r="P6" s="1"/>
-      <x:c r="Q6" s="1"/>
-      <x:c r="R6" s="1"/>
-      <x:c r="S6" s="1"/>
-      <x:c r="T6" s="1"/>
-      <x:c r="U6" s="1"/>
-      <x:c r="V6" s="1"/>
+      <x:c r="G6" s="4"/>
+      <x:c r="H6" s="4"/>
+      <x:c r="I6" s="5"/>
+      <x:c r="J6" s="5"/>
+      <x:c r="K6" s="5"/>
+      <x:c r="L6" s="5"/>
+      <x:c r="M6" s="5"/>
+      <x:c r="N6" s="5"/>
+      <x:c r="O6" s="5"/>
+      <x:c r="P6" s="6"/>
+      <x:c r="Q6" s="6"/>
+      <x:c r="R6" s="6"/>
+      <x:c r="S6" s="6"/>
+      <x:c r="T6" s="6"/>
+      <x:c r="U6" s="6"/>
+      <x:c r="V6" s="6"/>
       <x:c r="W6" s="1"/>
       <x:c r="X6" s="1"/>
       <x:c r="Y6" s="1"/>
@@ -1294,7 +1320,7 @@
     </x:row>
     <x:row r="7" spans="1:29">
       <x:c r="A7" s="2" t="s">
-        <x:v>11</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="B7" s="1"/>
       <x:c r="C7" s="1"/>
@@ -1329,20 +1355,20 @@
       <x:c r="A8" s="1" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B8" s="3"/>
-      <x:c r="C8" s="3"/>
-      <x:c r="D8" s="3"/>
-      <x:c r="E8" s="3"/>
-      <x:c r="F8" s="3"/>
-      <x:c r="G8" s="3"/>
-      <x:c r="H8" s="3"/>
-      <x:c r="I8" s="3"/>
-      <x:c r="J8" s="1"/>
-      <x:c r="K8" s="1"/>
-      <x:c r="L8" s="1"/>
-      <x:c r="M8" s="1"/>
-      <x:c r="N8" s="1"/>
-      <x:c r="O8" s="1"/>
+      <x:c r="B8" s="4"/>
+      <x:c r="C8" s="4"/>
+      <x:c r="D8" s="4"/>
+      <x:c r="E8" s="4"/>
+      <x:c r="F8" s="4"/>
+      <x:c r="G8" s="4"/>
+      <x:c r="H8" s="4"/>
+      <x:c r="I8" s="5"/>
+      <x:c r="J8" s="5"/>
+      <x:c r="K8" s="5"/>
+      <x:c r="L8" s="5"/>
+      <x:c r="M8" s="5"/>
+      <x:c r="N8" s="5"/>
+      <x:c r="O8" s="5"/>
       <x:c r="P8" s="1"/>
       <x:c r="Q8" s="1"/>
       <x:c r="R8" s="1"/>
@@ -1360,22 +1386,22 @@
     </x:row>
     <x:row r="9" spans="1:29">
       <x:c r="A9" s="1" t="s">
-        <x:v>21</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B9" s="3"/>
       <x:c r="C9" s="3"/>
-      <x:c r="D9" s="3"/>
-      <x:c r="E9" s="3"/>
-      <x:c r="F9" s="3"/>
-      <x:c r="G9" s="3"/>
-      <x:c r="H9" s="3"/>
-      <x:c r="I9" s="3"/>
-      <x:c r="J9" s="1"/>
-      <x:c r="K9" s="1"/>
-      <x:c r="L9" s="1"/>
-      <x:c r="M9" s="1"/>
-      <x:c r="N9" s="1"/>
-      <x:c r="O9" s="1"/>
+      <x:c r="D9" s="4"/>
+      <x:c r="E9" s="4"/>
+      <x:c r="F9" s="4"/>
+      <x:c r="G9" s="4"/>
+      <x:c r="H9" s="4"/>
+      <x:c r="I9" s="5"/>
+      <x:c r="J9" s="5"/>
+      <x:c r="K9" s="5"/>
+      <x:c r="L9" s="5"/>
+      <x:c r="M9" s="5"/>
+      <x:c r="N9" s="5"/>
+      <x:c r="O9" s="5"/>
       <x:c r="P9" s="1"/>
       <x:c r="Q9" s="1"/>
       <x:c r="R9" s="1"/>
@@ -1393,7 +1419,7 @@
     </x:row>
     <x:row r="10" spans="1:29">
       <x:c r="A10" s="2" t="s">
-        <x:v>10</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="B10" s="1"/>
       <x:c r="C10" s="1"/>
@@ -1426,29 +1452,29 @@
     </x:row>
     <x:row r="11" spans="1:29">
       <x:c r="A11" s="1" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B11" s="1"/>
-      <x:c r="C11" s="1"/>
-      <x:c r="D11" s="1"/>
-      <x:c r="E11" s="1"/>
-      <x:c r="F11" s="1"/>
-      <x:c r="G11" s="1"/>
-      <x:c r="H11" s="1"/>
-      <x:c r="I11" s="1"/>
-      <x:c r="J11" s="1"/>
-      <x:c r="K11" s="1"/>
-      <x:c r="L11" s="1"/>
-      <x:c r="M11" s="1"/>
-      <x:c r="N11" s="1"/>
-      <x:c r="O11" s="1"/>
-      <x:c r="P11" s="1"/>
-      <x:c r="Q11" s="1"/>
-      <x:c r="R11" s="1"/>
-      <x:c r="S11" s="1"/>
-      <x:c r="T11" s="1"/>
-      <x:c r="U11" s="1"/>
-      <x:c r="V11" s="1"/>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B11" s="4"/>
+      <x:c r="C11" s="4"/>
+      <x:c r="D11" s="4"/>
+      <x:c r="E11" s="4"/>
+      <x:c r="F11" s="4"/>
+      <x:c r="G11" s="4"/>
+      <x:c r="H11" s="4"/>
+      <x:c r="I11" s="5"/>
+      <x:c r="J11" s="5"/>
+      <x:c r="K11" s="5"/>
+      <x:c r="L11" s="5"/>
+      <x:c r="M11" s="5"/>
+      <x:c r="N11" s="5"/>
+      <x:c r="O11" s="5"/>
+      <x:c r="P11" s="3"/>
+      <x:c r="Q11" s="3"/>
+      <x:c r="R11" s="3"/>
+      <x:c r="S11" s="3"/>
+      <x:c r="T11" s="3"/>
+      <x:c r="U11" s="3"/>
+      <x:c r="V11" s="3"/>
       <x:c r="W11" s="1"/>
       <x:c r="X11" s="1"/>
       <x:c r="Y11" s="1"/>
@@ -1459,7 +1485,7 @@
     </x:row>
     <x:row r="12" spans="1:29">
       <x:c r="A12" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B12" s="1"/>
       <x:c r="C12" s="1"/>
@@ -1482,17 +1508,17 @@
       <x:c r="T12" s="1"/>
       <x:c r="U12" s="1"/>
       <x:c r="V12" s="1"/>
-      <x:c r="W12" s="1"/>
-      <x:c r="X12" s="1"/>
-      <x:c r="Y12" s="1"/>
-      <x:c r="Z12" s="1"/>
-      <x:c r="AA12" s="1"/>
-      <x:c r="AB12" s="1"/>
-      <x:c r="AC12" s="1"/>
+      <x:c r="W12" s="7"/>
+      <x:c r="X12" s="7"/>
+      <x:c r="Y12" s="7"/>
+      <x:c r="Z12" s="7"/>
+      <x:c r="AA12" s="7"/>
+      <x:c r="AB12" s="7"/>
+      <x:c r="AC12" s="7"/>
     </x:row>
     <x:row r="13" spans="1:29">
       <x:c r="A13" s="2" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B13" s="1"/>
       <x:c r="C13" s="1"/>
@@ -1530,24 +1556,24 @@
       <x:c r="B14" s="1"/>
       <x:c r="C14" s="1"/>
       <x:c r="D14" s="1"/>
-      <x:c r="E14" s="1"/>
-      <x:c r="F14" s="1"/>
-      <x:c r="G14" s="1"/>
-      <x:c r="H14" s="1"/>
-      <x:c r="I14" s="1"/>
-      <x:c r="J14" s="1"/>
-      <x:c r="K14" s="1"/>
-      <x:c r="L14" s="1"/>
-      <x:c r="M14" s="1"/>
-      <x:c r="N14" s="1"/>
-      <x:c r="O14" s="1"/>
-      <x:c r="P14" s="1"/>
-      <x:c r="Q14" s="1"/>
-      <x:c r="R14" s="1"/>
-      <x:c r="S14" s="1"/>
-      <x:c r="T14" s="1"/>
-      <x:c r="U14" s="1"/>
-      <x:c r="V14" s="1"/>
+      <x:c r="E14" s="4"/>
+      <x:c r="F14" s="4"/>
+      <x:c r="G14" s="4"/>
+      <x:c r="H14" s="4"/>
+      <x:c r="I14" s="5"/>
+      <x:c r="J14" s="5"/>
+      <x:c r="K14" s="5"/>
+      <x:c r="L14" s="5"/>
+      <x:c r="M14" s="5"/>
+      <x:c r="N14" s="5"/>
+      <x:c r="O14" s="5"/>
+      <x:c r="P14" s="3"/>
+      <x:c r="Q14" s="3"/>
+      <x:c r="R14" s="3"/>
+      <x:c r="S14" s="3"/>
+      <x:c r="T14" s="3"/>
+      <x:c r="U14" s="3"/>
+      <x:c r="V14" s="3"/>
       <x:c r="W14" s="1"/>
       <x:c r="X14" s="1"/>
       <x:c r="Y14" s="1"/>
@@ -1556,6 +1582,72 @@
       <x:c r="AB14" s="1"/>
       <x:c r="AC14" s="1"/>
     </x:row>
+    <x:row r="15" spans="1:29">
+      <x:c r="A15" s="9" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B15" s="10"/>
+      <x:c r="C15" s="10"/>
+      <x:c r="D15" s="10"/>
+      <x:c r="E15" s="10"/>
+      <x:c r="F15" s="10"/>
+      <x:c r="G15" s="10"/>
+      <x:c r="H15" s="10"/>
+      <x:c r="I15" s="10"/>
+      <x:c r="J15" s="10"/>
+      <x:c r="K15" s="10"/>
+      <x:c r="L15" s="10"/>
+      <x:c r="M15" s="10"/>
+      <x:c r="N15" s="10"/>
+      <x:c r="O15" s="10"/>
+      <x:c r="P15" s="10"/>
+      <x:c r="Q15" s="10"/>
+      <x:c r="R15" s="10"/>
+      <x:c r="S15" s="10"/>
+      <x:c r="T15" s="10"/>
+      <x:c r="U15" s="10"/>
+      <x:c r="V15" s="10"/>
+      <x:c r="W15" s="10"/>
+      <x:c r="X15" s="10"/>
+      <x:c r="Y15" s="10"/>
+      <x:c r="Z15" s="10"/>
+      <x:c r="AA15" s="10"/>
+      <x:c r="AB15" s="10"/>
+      <x:c r="AC15" s="10"/>
+    </x:row>
+    <x:row r="16" spans="1:29">
+      <x:c r="A16" s="1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B16" s="10"/>
+      <x:c r="C16" s="10"/>
+      <x:c r="D16" s="10"/>
+      <x:c r="E16" s="10"/>
+      <x:c r="F16" s="10"/>
+      <x:c r="G16" s="10"/>
+      <x:c r="H16" s="10"/>
+      <x:c r="I16" s="12"/>
+      <x:c r="J16" s="12"/>
+      <x:c r="K16" s="12"/>
+      <x:c r="L16" s="12"/>
+      <x:c r="M16" s="12"/>
+      <x:c r="N16" s="12"/>
+      <x:c r="O16" s="12"/>
+      <x:c r="P16" s="11"/>
+      <x:c r="Q16" s="11"/>
+      <x:c r="R16" s="11"/>
+      <x:c r="S16" s="11"/>
+      <x:c r="T16" s="11"/>
+      <x:c r="U16" s="11"/>
+      <x:c r="V16" s="11"/>
+      <x:c r="W16" s="10"/>
+      <x:c r="X16" s="10"/>
+      <x:c r="Y16" s="10"/>
+      <x:c r="Z16" s="10"/>
+      <x:c r="AA16" s="10"/>
+      <x:c r="AB16" s="10"/>
+      <x:c r="AC16" s="10"/>
+    </x:row>
   </x:sheetData>
   <x:mergeCells count="4">
     <x:mergeCell ref="B1:H1"/>
@@ -1563,7 +1655,7 @@
     <x:mergeCell ref="P1:V1"/>
     <x:mergeCell ref="W1:AC1"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51180553436279297" footer="0.51180553436279297"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51166665554046631" footer="0.51166665554046631"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>

<commit_message>
Modify: Gant Chart, Schedule summary
</commit_message>
<xml_diff>
--- a/Development Plan/Gant Chart.xlsx
+++ b/Development Plan/Gant Chart.xlsx
@@ -16,28 +16,58 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <x:si>
+    <x:t>허진수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>금</x:t>
+  </x:si>
+  <x:si>
+    <x:t>김현지</x:t>
+  </x:si>
+  <x:si>
+    <x:t>이연수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>목</x:t>
+  </x:si>
+  <x:si>
+    <x:t>화</x:t>
+  </x:si>
+  <x:si>
+    <x:t>토</x:t>
+  </x:si>
+  <x:si>
+    <x:t>일</x:t>
+  </x:si>
+  <x:si>
+    <x:t>월</x:t>
+  </x:si>
+  <x:si>
+    <x:t>수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2주차 (05.30 ~ 06.05)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1주차 (05.23 ~ 29)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3주차 (06.06 ~ 12)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>카드리딘, 허진수, 김현지, 이연수</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4주차 (06.13 ~ 19)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>알고리즘, 모델 자료 수집</x:t>
+  </x:si>
+  <x:si>
     <x:t>댓글의 긍정/부정 분석</x:t>
   </x:si>
   <x:si>
-    <x:t>화</x:t>
-  </x:si>
-  <x:si>
-    <x:t>허진수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>토</x:t>
-  </x:si>
-  <x:si>
-    <x:t>금</x:t>
-  </x:si>
-  <x:si>
-    <x:t>김현지</x:t>
-  </x:si>
-  <x:si>
-    <x:t>목</x:t>
-  </x:si>
-  <x:si>
-    <x:t>일</x:t>
+    <x:t>개발 환경 Setting</x:t>
   </x:si>
   <x:si>
     <x:t>Page 제작</x:t>
@@ -46,56 +76,26 @@
     <x:t>카드리딘</x:t>
   </x:si>
   <x:si>
-    <x:t>2주차 (05.30 ~ 06.05)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1주차 (05.23 ~ 29)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>3주차 (06.06 ~ 12)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>4주차 (06.13 ~ 19)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>카드리딘, 허진수, 김현지, 이연수</x:t>
-  </x:si>
-  <x:si>
     <x:t>Page 디자인</x:t>
   </x:si>
   <x:si>
+    <x:t>Rest API 생성</x:t>
+  </x:si>
+  <x:si>
     <x:t>크롤링한 데이터 관리</x:t>
   </x:si>
   <x:si>
+    <x:t>영상 댓글 크롤링</x:t>
+  </x:si>
+  <x:si>
     <x:t>워드 클라우드 제작</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Rest API 생성</x:t>
-  </x:si>
-  <x:si>
-    <x:t>영상 댓글 크롤링</x:t>
-  </x:si>
-  <x:si>
-    <x:t>수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>이연수</x:t>
-  </x:si>
-  <x:si>
-    <x:t>월</x:t>
-  </x:si>
-  <x:si>
-    <x:t>알고리즘, 모델 자료 수집</x:t>
-  </x:si>
-  <x:si>
-    <x:t>개발 환경 Setting</x:t>
   </x:si>
 </x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <x:styleSheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:fonts count="9">
+  <x:fonts count="8">
     <x:font>
       <x:name val="돋움"/>
       <x:sz val="11"/>
@@ -130,12 +130,6 @@
       <x:name val="돋움"/>
       <x:sz val="11"/>
       <x:color rgb="ff000000"/>
-      <x:b val="1"/>
-    </x:font>
-    <x:font>
-      <x:name val="돋움"/>
-      <x:sz val="11"/>
-      <x:color rgb="ffff0000"/>
       <x:b val="1"/>
     </x:font>
     <x:font>
@@ -356,6 +350,18 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <x:xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <x:alignment horizontal="general" vertical="center"/>
+    </x:xf>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1" hs:applyExtension="1">
@@ -369,18 +375,6 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
-    <x:xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <x:alignment horizontal="general" vertical="center"/>
-    </x:xf>
   </x:cellXfs>
   <x:cellStyles count="6">
     <x:cellStyle xfId="15" builtinId="5" iLevel="0"/>
@@ -396,7 +390,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -479,7 +472,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -514,7 +506,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -559,7 +550,6 @@
           <x:font hs:extension="1">
             <x:color rgb="ffffffff"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -603,7 +593,6 @@
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
             <x:color rgb="ff000000"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -687,8 +676,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
+            <x:color indexed="64"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -699,6 +688,7 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
+            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
         </x:dxf>
@@ -708,8 +698,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
+            <x:color indexed="64"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -725,6 +715,7 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
+            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -739,8 +730,8 @@
       <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
         <x:dxf hs:applyExtension="1">
           <x:font hs:extension="1">
+            <x:color indexed="64"/>
             <x:b val="1"/>
-            <hs:useFontSpace val="0"/>
             <hs:size val="0"/>
             <hs:ratio val="0"/>
             <hs:spacing val="0"/>
@@ -756,6 +747,7 @@
       <mc:Fallback>
         <x:dxf>
           <x:font>
+            <x:color indexed="64"/>
             <x:b val="1"/>
           </x:font>
           <x:border>
@@ -1051,7 +1043,7 @@
   <x:dimension ref="A1:AC16"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="Q7" activeCellId="0" sqref="Q7:Q7"/>
+      <x:selection activeCell="M6" activeCellId="0" sqref="M6:M6"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.550000000000001"/>
@@ -1062,125 +1054,125 @@
   <x:sheetData>
     <x:row r="1" spans="1:29">
       <x:c r="A1" s="3"/>
-      <x:c r="B1" s="8" t="s">
+      <x:c r="B1" s="12" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="C1" s="8"/>
-      <x:c r="D1" s="8"/>
-      <x:c r="E1" s="8"/>
-      <x:c r="F1" s="8"/>
-      <x:c r="G1" s="8"/>
-      <x:c r="H1" s="8"/>
-      <x:c r="I1" s="8" t="s">
+      <x:c r="C1" s="12"/>
+      <x:c r="D1" s="12"/>
+      <x:c r="E1" s="12"/>
+      <x:c r="F1" s="12"/>
+      <x:c r="G1" s="12"/>
+      <x:c r="H1" s="12"/>
+      <x:c r="I1" s="12" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="J1" s="8"/>
-      <x:c r="K1" s="8"/>
-      <x:c r="L1" s="8"/>
-      <x:c r="M1" s="8"/>
-      <x:c r="N1" s="8"/>
-      <x:c r="O1" s="8"/>
-      <x:c r="P1" s="8" t="s">
+      <x:c r="J1" s="12"/>
+      <x:c r="K1" s="12"/>
+      <x:c r="L1" s="12"/>
+      <x:c r="M1" s="12"/>
+      <x:c r="N1" s="12"/>
+      <x:c r="O1" s="12"/>
+      <x:c r="P1" s="12" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="Q1" s="8"/>
-      <x:c r="R1" s="8"/>
-      <x:c r="S1" s="8"/>
-      <x:c r="T1" s="8"/>
-      <x:c r="U1" s="8"/>
-      <x:c r="V1" s="8"/>
-      <x:c r="W1" s="8" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="X1" s="8"/>
-      <x:c r="Y1" s="8"/>
-      <x:c r="Z1" s="8"/>
-      <x:c r="AA1" s="8"/>
-      <x:c r="AB1" s="8"/>
-      <x:c r="AC1" s="8"/>
+      <x:c r="Q1" s="12"/>
+      <x:c r="R1" s="12"/>
+      <x:c r="S1" s="12"/>
+      <x:c r="T1" s="12"/>
+      <x:c r="U1" s="12"/>
+      <x:c r="V1" s="12"/>
+      <x:c r="W1" s="12" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="X1" s="12"/>
+      <x:c r="Y1" s="12"/>
+      <x:c r="Z1" s="12"/>
+      <x:c r="AA1" s="12"/>
+      <x:c r="AB1" s="12"/>
+      <x:c r="AC1" s="12"/>
     </x:row>
     <x:row r="2" spans="1:29">
       <x:c r="A2" s="1"/>
       <x:c r="B2" s="4" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C2" s="4" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D2" s="4" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E2" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F2" s="4" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="D2" s="4" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="E2" s="4" t="s">
+      <x:c r="G2" s="4" t="s">
         <x:v>6</x:v>
-      </x:c>
-      <x:c r="F2" s="4" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="G2" s="4" t="s">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="H2" s="4" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="I2" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="J2" s="5" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="K2" s="5" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="L2" s="5" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="M2" s="5" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="K2" s="5" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="L2" s="5" t="s">
+      <x:c r="N2" s="5" t="s">
         <x:v>6</x:v>
-      </x:c>
-      <x:c r="M2" s="5" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="N2" s="5" t="s">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="O2" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="P2" s="6" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="Q2" s="6" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="R2" s="6" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="S2" s="6" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="T2" s="6" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="R2" s="6" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="S2" s="6" t="s">
+      <x:c r="U2" s="6" t="s">
         <x:v>6</x:v>
-      </x:c>
-      <x:c r="T2" s="6" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="U2" s="6" t="s">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="V2" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
       <x:c r="W2" s="7" t="s">
-        <x:v>22</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="X2" s="7" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="Y2" s="7" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="Z2" s="7" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="AA2" s="7" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="Y2" s="7" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="Z2" s="7" t="s">
+      <x:c r="AB2" s="7" t="s">
         <x:v>6</x:v>
-      </x:c>
-      <x:c r="AA2" s="7" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="AB2" s="7" t="s">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="AC2" s="7" t="s">
         <x:v>7</x:v>
@@ -1188,7 +1180,7 @@
     </x:row>
     <x:row r="3" spans="1:29">
       <x:c r="A3" s="2" t="s">
-        <x:v>9</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B3" s="1"/>
       <x:c r="C3" s="1"/>
@@ -1221,7 +1213,7 @@
     </x:row>
     <x:row r="4" spans="1:29">
       <x:c r="A4" s="1" t="s">
-        <x:v>24</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B4" s="4"/>
       <x:c r="C4" s="4"/>
@@ -1254,7 +1246,7 @@
     </x:row>
     <x:row r="5" spans="1:29">
       <x:c r="A5" s="1" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B5" s="3"/>
       <x:c r="C5" s="3"/>
@@ -1287,7 +1279,7 @@
     </x:row>
     <x:row r="6" spans="1:29">
       <x:c r="A6" s="1" t="s">
-        <x:v>23</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B6" s="1"/>
       <x:c r="C6" s="1"/>
@@ -1353,7 +1345,7 @@
     </x:row>
     <x:row r="8" spans="1:29">
       <x:c r="A8" s="1" t="s">
-        <x:v>15</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="B8" s="4"/>
       <x:c r="C8" s="4"/>
@@ -1386,7 +1378,7 @@
     </x:row>
     <x:row r="9" spans="1:29">
       <x:c r="A9" s="1" t="s">
-        <x:v>8</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="B9" s="3"/>
       <x:c r="C9" s="3"/>
@@ -1419,7 +1411,7 @@
     </x:row>
     <x:row r="10" spans="1:29">
       <x:c r="A10" s="2" t="s">
-        <x:v>5</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B10" s="1"/>
       <x:c r="C10" s="1"/>
@@ -1452,7 +1444,7 @@
     </x:row>
     <x:row r="11" spans="1:29">
       <x:c r="A11" s="1" t="s">
-        <x:v>19</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B11" s="4"/>
       <x:c r="C11" s="4"/>
@@ -1485,7 +1477,7 @@
     </x:row>
     <x:row r="12" spans="1:29">
       <x:c r="A12" s="1" t="s">
-        <x:v>17</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="B12" s="1"/>
       <x:c r="C12" s="1"/>
@@ -1518,7 +1510,7 @@
     </x:row>
     <x:row r="13" spans="1:29">
       <x:c r="A13" s="2" t="s">
-        <x:v>21</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="B13" s="1"/>
       <x:c r="C13" s="1"/>
@@ -1551,7 +1543,7 @@
     </x:row>
     <x:row r="14" spans="1:29">
       <x:c r="A14" s="1" t="s">
-        <x:v>16</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="B14" s="1"/>
       <x:c r="C14" s="1"/>
@@ -1583,70 +1575,70 @@
       <x:c r="AC14" s="1"/>
     </x:row>
     <x:row r="15" spans="1:29">
-      <x:c r="A15" s="9" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B15" s="10"/>
-      <x:c r="C15" s="10"/>
-      <x:c r="D15" s="10"/>
-      <x:c r="E15" s="10"/>
-      <x:c r="F15" s="10"/>
-      <x:c r="G15" s="10"/>
-      <x:c r="H15" s="10"/>
-      <x:c r="I15" s="10"/>
-      <x:c r="J15" s="10"/>
-      <x:c r="K15" s="10"/>
-      <x:c r="L15" s="10"/>
-      <x:c r="M15" s="10"/>
-      <x:c r="N15" s="10"/>
-      <x:c r="O15" s="10"/>
-      <x:c r="P15" s="10"/>
-      <x:c r="Q15" s="10"/>
-      <x:c r="R15" s="10"/>
-      <x:c r="S15" s="10"/>
-      <x:c r="T15" s="10"/>
-      <x:c r="U15" s="10"/>
-      <x:c r="V15" s="10"/>
-      <x:c r="W15" s="10"/>
-      <x:c r="X15" s="10"/>
-      <x:c r="Y15" s="10"/>
-      <x:c r="Z15" s="10"/>
-      <x:c r="AA15" s="10"/>
-      <x:c r="AB15" s="10"/>
-      <x:c r="AC15" s="10"/>
+      <x:c r="A15" s="8" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B15" s="9"/>
+      <x:c r="C15" s="9"/>
+      <x:c r="D15" s="9"/>
+      <x:c r="E15" s="9"/>
+      <x:c r="F15" s="9"/>
+      <x:c r="G15" s="9"/>
+      <x:c r="H15" s="9"/>
+      <x:c r="I15" s="9"/>
+      <x:c r="J15" s="9"/>
+      <x:c r="K15" s="9"/>
+      <x:c r="L15" s="9"/>
+      <x:c r="M15" s="9"/>
+      <x:c r="N15" s="9"/>
+      <x:c r="O15" s="9"/>
+      <x:c r="P15" s="9"/>
+      <x:c r="Q15" s="9"/>
+      <x:c r="R15" s="9"/>
+      <x:c r="S15" s="9"/>
+      <x:c r="T15" s="9"/>
+      <x:c r="U15" s="9"/>
+      <x:c r="V15" s="9"/>
+      <x:c r="W15" s="9"/>
+      <x:c r="X15" s="9"/>
+      <x:c r="Y15" s="9"/>
+      <x:c r="Z15" s="9"/>
+      <x:c r="AA15" s="9"/>
+      <x:c r="AB15" s="9"/>
+      <x:c r="AC15" s="9"/>
     </x:row>
     <x:row r="16" spans="1:29">
       <x:c r="A16" s="1" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="B16" s="10"/>
-      <x:c r="C16" s="10"/>
-      <x:c r="D16" s="10"/>
-      <x:c r="E16" s="10"/>
-      <x:c r="F16" s="10"/>
-      <x:c r="G16" s="10"/>
-      <x:c r="H16" s="10"/>
-      <x:c r="I16" s="12"/>
-      <x:c r="J16" s="12"/>
-      <x:c r="K16" s="12"/>
-      <x:c r="L16" s="12"/>
-      <x:c r="M16" s="12"/>
-      <x:c r="N16" s="12"/>
-      <x:c r="O16" s="12"/>
-      <x:c r="P16" s="11"/>
-      <x:c r="Q16" s="11"/>
-      <x:c r="R16" s="11"/>
-      <x:c r="S16" s="11"/>
-      <x:c r="T16" s="11"/>
-      <x:c r="U16" s="11"/>
-      <x:c r="V16" s="11"/>
-      <x:c r="W16" s="10"/>
-      <x:c r="X16" s="10"/>
-      <x:c r="Y16" s="10"/>
-      <x:c r="Z16" s="10"/>
-      <x:c r="AA16" s="10"/>
-      <x:c r="AB16" s="10"/>
-      <x:c r="AC16" s="10"/>
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B16" s="9"/>
+      <x:c r="C16" s="9"/>
+      <x:c r="D16" s="9"/>
+      <x:c r="E16" s="9"/>
+      <x:c r="F16" s="9"/>
+      <x:c r="G16" s="9"/>
+      <x:c r="H16" s="9"/>
+      <x:c r="I16" s="11"/>
+      <x:c r="J16" s="11"/>
+      <x:c r="K16" s="11"/>
+      <x:c r="L16" s="11"/>
+      <x:c r="M16" s="11"/>
+      <x:c r="N16" s="11"/>
+      <x:c r="O16" s="11"/>
+      <x:c r="P16" s="10"/>
+      <x:c r="Q16" s="10"/>
+      <x:c r="R16" s="10"/>
+      <x:c r="S16" s="10"/>
+      <x:c r="T16" s="10"/>
+      <x:c r="U16" s="10"/>
+      <x:c r="V16" s="10"/>
+      <x:c r="W16" s="9"/>
+      <x:c r="X16" s="9"/>
+      <x:c r="Y16" s="9"/>
+      <x:c r="Z16" s="9"/>
+      <x:c r="AA16" s="9"/>
+      <x:c r="AB16" s="9"/>
+      <x:c r="AC16" s="9"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="4">
@@ -1655,7 +1647,7 @@
     <x:mergeCell ref="P1:V1"/>
     <x:mergeCell ref="W1:AC1"/>
   </x:mergeCells>
-  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51166665554046631" footer="0.51166665554046631"/>
+  <x:pageMargins left="0.74805557727813721" right="0.74805557727813721" top="0.98430556058883667" bottom="0.98430556058883667" header="0.51152777671813965" footer="0.51152777671813965"/>
   <x:pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" useFirstPageNumber="0" horizontalDpi="600" verticalDpi="600" copies="1"/>
 </x:worksheet>
 </file>
</xml_diff>